<commit_message>
update assignment 4 and add semester project
</commit_message>
<xml_diff>
--- a/Assignment4/Assignment4.xlsx
+++ b/Assignment4/Assignment4.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -477,19 +477,59 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>speedywait</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>ripenmusical</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>images/pp2.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>locksignal</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>opticianblazer</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>images/pp4.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
         <v>5</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B5" t="inlineStr">
         <is>
           <t>centurysyrup</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>soybeanremain</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t>images/pp6.png</t>
         </is>

</xml_diff>